<commit_message>
Changed template and payroll API
Fixed some bugs with copying, added payroll entry API to database.
Added code to change the dates in the excel file
Filling out grand total at bottom of template
You can now finalize the file and it renames it to the period end date
</commit_message>
<xml_diff>
--- a/timecard-system/Payroll-Files/Template.xlsx
+++ b/timecard-system/Payroll-Files/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt-Admin\Desktop\Time_Guard\timecard-system\Payroll-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30843746-47CE-4BB4-8DB9-0C8A5A56F80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC63560-5897-4480-831A-51B1798D283C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E656B24C-75A0-4820-98ED-4E6737654023}"/>
+    <workbookView xWindow="7290" yWindow="2220" windowWidth="21600" windowHeight="11385" xr2:uid="{E656B24C-75A0-4820-98ED-4E6737654023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -291,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -307,7 +307,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -666,7 +665,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -680,69 +679,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11">
+      <c r="B1" s="10">
         <v>270113</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="H1" s="9" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="H1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="10">
-        <v>45534</v>
-      </c>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="H2" s="9" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="H2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="10">
-        <v>45527</v>
-      </c>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="H3" s="9" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="H3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="10">
-        <v>45525</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="5" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -777,315 +759,301 @@
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
     </row>
     <row r="17" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
     </row>
     <row r="18" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11" ht="64.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
     </row>
     <row r="24" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="14">
-        <v>123.12</v>
-      </c>
-      <c r="C25" s="14">
-        <v>123.12</v>
-      </c>
-      <c r="D25" s="14">
-        <v>123.12</v>
-      </c>
-      <c r="E25" s="14">
-        <v>123.12</v>
-      </c>
-      <c r="F25" s="14">
-        <v>123.12</v>
-      </c>
-      <c r="G25" s="14">
-        <v>123.12</v>
-      </c>
-      <c r="H25" s="14">
-        <v>123.12</v>
-      </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>